<commit_message>
respuesta procesada, print estado registro facturas
</commit_message>
<xml_diff>
--- a/data/Copia de Ventas_0002_00_240411_.xlsx
+++ b/data/Copia de Ventas_0002_00_240411_.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>NumFactura</t>
   </si>
@@ -123,16 +123,7 @@
     <t>PAPP ZSOLT</t>
   </si>
   <si>
-    <t>A19252</t>
-  </si>
-  <si>
-    <t>A19253</t>
-  </si>
-  <si>
-    <t>A19254</t>
-  </si>
-  <si>
-    <t>A19255</t>
+    <t>A19260</t>
   </si>
 </sst>
 </file>
@@ -466,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -632,165 +623,6 @@
         <v>344</v>
       </c>
       <c r="AF2">
-        <v>430000344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="1">
-        <v>65.52</v>
-      </c>
-      <c r="F3" s="1">
-        <v>21</v>
-      </c>
-      <c r="G3" s="1">
-        <v>13.76</v>
-      </c>
-      <c r="J3" s="1">
-        <v>12.25</v>
-      </c>
-      <c r="K3" s="1">
-        <v>10</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1.23</v>
-      </c>
-      <c r="T3" s="1">
-        <v>20.83</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <v>0</v>
-      </c>
-      <c r="W3" s="1">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="2">
-        <v>344</v>
-      </c>
-      <c r="AF3">
-        <v>430000344</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="1">
-        <v>65.52</v>
-      </c>
-      <c r="F4" s="1">
-        <v>21</v>
-      </c>
-      <c r="G4" s="1">
-        <v>13.76</v>
-      </c>
-      <c r="J4" s="1">
-        <v>12.25</v>
-      </c>
-      <c r="K4" s="1">
-        <v>10</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1.23</v>
-      </c>
-      <c r="T4" s="1">
-        <v>20.83</v>
-      </c>
-      <c r="U4" s="1">
-        <v>0</v>
-      </c>
-      <c r="V4" s="1">
-        <v>0</v>
-      </c>
-      <c r="W4" s="1">
-        <v>0</v>
-      </c>
-      <c r="X4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>344</v>
-      </c>
-      <c r="AF4">
-        <v>430000344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="1">
-        <v>65.52</v>
-      </c>
-      <c r="F5" s="1">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1">
-        <v>13.76</v>
-      </c>
-      <c r="J5" s="1">
-        <v>12.25</v>
-      </c>
-      <c r="K5" s="1">
-        <v>10</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1.23</v>
-      </c>
-      <c r="T5" s="1">
-        <v>20.83</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0</v>
-      </c>
-      <c r="V5" s="1">
-        <v>0</v>
-      </c>
-      <c r="W5" s="1">
-        <v>0</v>
-      </c>
-      <c r="X5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>344</v>
-      </c>
-      <c r="AF5">
         <v>430000344</v>
       </c>
     </row>

</xml_diff>

<commit_message>
procesar mensaje respuesta correcto
</commit_message>
<xml_diff>
--- a/data/Copia de Ventas_0002_00_240411_.xlsx
+++ b/data/Copia de Ventas_0002_00_240411_.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>NumFactura</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>A19260</t>
+  </si>
+  <si>
+    <t>A19262</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -590,7 +593,7 @@
         <v>65.52</v>
       </c>
       <c r="F2" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1">
         <v>13.76</v>
@@ -623,11 +626,65 @@
         <v>344</v>
       </c>
       <c r="AF2">
+        <v>430000344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1">
+        <v>65.52</v>
+      </c>
+      <c r="F3" s="1">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1">
+        <v>13.76</v>
+      </c>
+      <c r="J3" s="1">
+        <v>12.25</v>
+      </c>
+      <c r="K3" s="1">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="T3" s="1">
+        <v>20.83</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>344</v>
+      </c>
+      <c r="AF3">
         <v>430000344</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>